<commit_message>
feat : solucion al promotor extra en promotores
</commit_message>
<xml_diff>
--- a/ejemplo_seccional.xlsx
+++ b/ejemplo_seccional.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\codigos\ixmicheck\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281B0852-4F65-4867-877B-222AD1D053DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96AD1601-E3E7-4571-8FA1-F5FC64A1DB92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3765" yWindow="3765" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4110" yWindow="4110" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Registrados" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
   <si>
     <t>Nombre Completo</t>
   </si>
@@ -181,19 +194,10 @@
     <t>DANIELA FABIOLA ISIDRO CRUZ</t>
   </si>
   <si>
-    <t>TOTAL PROMOVIDOS</t>
-  </si>
-  <si>
     <t>No Total.</t>
   </si>
   <si>
     <t>No. Promotor</t>
-  </si>
-  <si>
-    <t>TOTAL ASISTENTES</t>
-  </si>
-  <si>
-    <t>EFECTIVIDAD DE MOVILIZACIÓN</t>
   </si>
   <si>
     <t>SECCIONAL 0591 El maye</t>
@@ -203,7 +207,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -227,31 +231,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -294,12 +275,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -325,11 +300,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -364,32 +338,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -726,10 +681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -744,21 +699,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
+      <c r="A1" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>55</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>0</v>
@@ -772,7 +727,7 @@
       <c r="F2" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G2" s="20"/>
+      <c r="G2" s="16"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
@@ -1054,7 +1009,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -1070,141 +1025,9 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="42" x14ac:dyDescent="0.25">
-      <c r="B19" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" s="18">
-        <v>15</v>
-      </c>
-      <c r="D19" s="17"/>
-      <c r="E19" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="F19" s="19">
-        <v>4</v>
-      </c>
-      <c r="G19" s="21" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="16">
-        <v>3</v>
-      </c>
-      <c r="D20" s="17"/>
-      <c r="E20" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="F20" s="16">
-        <v>3</v>
-      </c>
-      <c r="G20" s="22">
-        <f>F20/C20*1</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="16">
-        <v>6</v>
-      </c>
-      <c r="D21" s="17"/>
-      <c r="E21" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="F21" s="16">
-        <v>1</v>
-      </c>
-      <c r="G21" s="22">
-        <f t="shared" ref="G21:G25" si="0">F21/C21*1</f>
-        <v>0.16666666666666666</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C22" s="16">
-        <v>1</v>
-      </c>
-      <c r="D22" s="17"/>
-      <c r="E22" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="F22" s="16">
-        <v>1</v>
-      </c>
-      <c r="G22" s="22">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="16">
-        <v>2</v>
-      </c>
-      <c r="D23" s="17"/>
-      <c r="E23" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="F23" s="16">
-        <v>1</v>
-      </c>
-      <c r="G23" s="22">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" s="16">
-        <v>2</v>
-      </c>
-      <c r="D24" s="17"/>
-      <c r="E24" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="F24" s="16">
-        <v>2</v>
-      </c>
-      <c r="G24" s="22">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="C25" s="16">
-        <v>1</v>
-      </c>
-      <c r="D25" s="17"/>
-      <c r="E25" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="F25" s="16">
-        <v>0</v>
-      </c>
-      <c r="G25" s="16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B56:F75">
-    <sortCondition ref="F56:F75"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B49:F68">
+    <sortCondition ref="F49:F68"/>
   </sortState>
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>

</xml_diff>